<commit_message>
Product Backlog (Estimativa) e ATAS
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Backlog_TecnoSolo.xlsx
+++ b/sprint_grupo7/TI/Backlog_TecnoSolo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PI\sprint_02\sprint_grupo7\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9AA08CB-9620-4030-BC39-9F2FFECEF0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F02A67F-2094-45D5-A09F-4B61851800D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{04C4E037-2DBA-466C-9AD1-F933304BD8CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04C4E037-2DBA-466C-9AD1-F933304BD8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Requisito</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>Essencial+[@Descrição]</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>GG</t>
   </si>
 </sst>
 </file>
@@ -1488,24 +1500,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6281045-9D37-4D83-95EA-DA78B31E06C6}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="A20:B20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" customWidth="1"/>
-    <col min="2" max="2" width="56.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="50.7265625" customWidth="1"/>
-    <col min="7" max="8" width="18.7265625" customWidth="1"/>
-    <col min="9" max="10" width="10.26953125" customWidth="1"/>
-    <col min="16" max="16" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="56.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="50.77734375" customWidth="1"/>
+    <col min="7" max="8" width="18.77734375" customWidth="1"/>
+    <col min="9" max="10" width="10.21875" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1543,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="58.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1544,8 +1556,12 @@
       <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="11"/>
+      <c r="E2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="11">
+        <v>13</v>
+      </c>
       <c r="G2" s="25"/>
       <c r="H2" s="11"/>
       <c r="P2" s="32" t="s">
@@ -1553,7 +1569,7 @@
       </c>
       <c r="Q2" s="33"/>
     </row>
-    <row r="3" spans="1:17" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="47.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -1566,8 +1582,12 @@
       <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="11">
+        <v>8</v>
+      </c>
       <c r="G3" s="25"/>
       <c r="H3" s="11"/>
       <c r="P3" s="34" t="s">
@@ -1575,7 +1595,7 @@
       </c>
       <c r="Q3" s="29"/>
     </row>
-    <row r="4" spans="1:17" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>52</v>
       </c>
@@ -1588,8 +1608,12 @@
       <c r="D4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="11">
+        <v>5</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="P4" s="34" t="s">
@@ -1597,7 +1621,7 @@
       </c>
       <c r="Q4" s="29"/>
     </row>
-    <row r="5" spans="1:17" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1610,8 +1634,12 @@
       <c r="D5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="11">
+        <v>13</v>
+      </c>
       <c r="G5" s="25"/>
       <c r="H5" s="11"/>
       <c r="P5" s="34" t="s">
@@ -1619,7 +1647,7 @@
       </c>
       <c r="Q5" s="29"/>
     </row>
-    <row r="6" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1632,8 +1660,12 @@
       <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="11">
+        <v>8</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="11"/>
       <c r="I6" s="1"/>
@@ -1642,7 +1674,7 @@
       </c>
       <c r="Q6" s="30"/>
     </row>
-    <row r="7" spans="1:17" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="38.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1655,8 +1687,12 @@
       <c r="D7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="11">
+        <v>13</v>
+      </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="2"/>
@@ -1665,7 +1701,7 @@
       </c>
       <c r="Q7" s="29"/>
     </row>
-    <row r="8" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
@@ -1678,8 +1714,12 @@
       <c r="D8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="11">
+        <v>8</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="2"/>
@@ -1688,7 +1728,7 @@
       </c>
       <c r="Q8" s="31"/>
     </row>
-    <row r="9" spans="1:17" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="47.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
@@ -1701,13 +1741,17 @@
       <c r="D9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="11">
+        <v>21</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>18</v>
       </c>
@@ -1720,13 +1764,17 @@
       <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="11">
+        <v>21</v>
+      </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>40</v>
       </c>
@@ -1739,13 +1787,17 @@
       <c r="D11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="11">
+        <v>21</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>38</v>
       </c>
@@ -1758,13 +1810,17 @@
       <c r="D12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="11">
+        <v>5</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>41</v>
       </c>
@@ -1777,13 +1833,17 @@
       <c r="D13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="11">
+        <v>5</v>
+      </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>43</v>
       </c>
@@ -1796,12 +1856,16 @@
       <c r="D14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="25">
+        <v>8</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>45</v>
       </c>
@@ -1814,12 +1878,16 @@
       <c r="D15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="25">
+        <v>5</v>
+      </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:17" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>48</v>
       </c>
@@ -1832,12 +1900,16 @@
       <c r="D16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="11">
+        <v>5</v>
+      </c>
       <c r="G16" s="25"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>51</v>
       </c>
@@ -1850,12 +1922,12 @@
       <c r="D17" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>54</v>
       </c>
@@ -1868,12 +1940,16 @@
       <c r="D18" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="25"/>
+      <c r="E18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="25">
+        <v>13</v>
+      </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="50.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>56</v>
       </c>
@@ -1886,12 +1962,16 @@
       <c r="D19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="11">
+        <v>13</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="54.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>58</v>
       </c>
@@ -1905,19 +1985,19 @@
       <c r="G20" s="25"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E29" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizando product backlog Sprint2 B
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Backlog_TecnoSolo.xlsx
+++ b/sprint_grupo7/TI/Backlog_TecnoSolo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PI\sprint_02\sprint_grupo7\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Desktop\Faculdade\Pesquisa e Inovação\sprint_02\sprint_grupo7\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F02A67F-2094-45D5-A09F-4B61851800D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968B2656-40DA-4CD4-9972-29F2B50E4BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04C4E037-2DBA-466C-9AD1-F933304BD8CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{04C4E037-2DBA-466C-9AD1-F933304BD8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>Requisito</t>
   </si>
@@ -104,9 +93,6 @@
     <t>Botões: recursos; sobre nós; sua conta; suporte; rede social. Campo email para receber informações da plataforma.</t>
   </si>
   <si>
-    <t>Botões: recursos; suporte; comece já; são redirecionamento de página.</t>
-  </si>
-  <si>
     <t>Botão: Recursos; para redirecionar para recursos.</t>
   </si>
   <si>
@@ -116,9 +102,6 @@
     <t>Campos: Foto de Perfil; Plano de Fundo; Nome; CPF/CNPJ; Email; Alteral Senha; Repetir Senha; todos tem a ação de atualizar.</t>
   </si>
   <si>
-    <t>Vai receber os campos: email e uma permissão para receber atualizações sobre a nossa plataforma; nome completo; nome de usuário; senha com confirmação e validação da mesma;  CPF/CNPJ; data de nascimento; url que redireciona para tela login;</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -228,6 +211,27 @@
   </si>
   <si>
     <t>GG</t>
+  </si>
+  <si>
+    <t>Vai receber os campos: email e  senha com confirmação e validação da mesma; nome completo; CNPJ; telefone; nome da empresa; CEP; UF; cidade; bairro; rua e complemento.</t>
+  </si>
+  <si>
+    <t>Botões: recursos; suporte; home, sobre nós, simulador financeiro e conta</t>
+  </si>
+  <si>
+    <t>SP2 B</t>
+  </si>
+  <si>
+    <t>SP2 C</t>
+  </si>
+  <si>
+    <t>SP2 A</t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>SP2 D</t>
   </si>
 </sst>
 </file>
@@ -1500,24 +1504,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6281045-9D37-4D83-95EA-DA78B31E06C6}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="56.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="50.77734375" customWidth="1"/>
-    <col min="7" max="8" width="18.77734375" customWidth="1"/>
-    <col min="9" max="10" width="10.21875" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="10" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1531,24 +1535,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="58.05" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>7</v>
@@ -1557,19 +1561,21 @@
         <v>8</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="11">
         <v>13</v>
       </c>
       <c r="G2" s="25"/>
-      <c r="H2" s="11"/>
+      <c r="H2" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="33"/>
     </row>
-    <row r="3" spans="1:17" ht="47.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -1583,24 +1589,26 @@
         <v>8</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="11">
         <v>8</v>
       </c>
       <c r="G3" s="25"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="P3" s="34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="29"/>
     </row>
-    <row r="4" spans="1:17" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="42.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>7</v>
@@ -1609,24 +1617,26 @@
         <v>10</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="H4" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="P4" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="29"/>
     </row>
-    <row r="5" spans="1:17" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="44.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>7</v>
@@ -1635,19 +1645,21 @@
         <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="11">
         <v>13</v>
       </c>
       <c r="G5" s="25"/>
-      <c r="H5" s="11"/>
+      <c r="H5" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="P5" s="34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="29"/>
     </row>
-    <row r="6" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1661,20 +1673,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F6" s="11">
         <v>8</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="P6" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="30"/>
     </row>
-    <row r="7" spans="1:17" ht="38.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1688,25 +1702,27 @@
         <v>15</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="11">
         <v>13</v>
       </c>
       <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="H7" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="P7" s="34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="29"/>
     </row>
-    <row r="8" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>7</v>
@@ -1715,20 +1731,22 @@
         <v>15</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" s="11">
         <v>8</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="P8" s="35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="31"/>
     </row>
-    <row r="9" spans="1:17" ht="47.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
@@ -1742,21 +1760,23 @@
         <v>8</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" s="11">
         <v>21</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>7</v>
@@ -1765,18 +1785,20 @@
         <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" s="11">
         <v>21</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>19</v>
@@ -1788,21 +1810,23 @@
         <v>8</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="11">
         <v>21</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>7</v>
@@ -1811,113 +1835,123 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14" s="25">
         <v>8</v>
       </c>
       <c r="G14" s="11"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:17" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>47</v>
-      </c>
       <c r="C15" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15" s="25">
         <v>5</v>
       </c>
       <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:17" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" s="11">
         <v>5</v>
       </c>
       <c r="G16" s="25"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>53</v>
-      </c>
       <c r="C17" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>8</v>
@@ -1925,59 +1959,65 @@
       <c r="E17" s="9"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18" s="25">
         <v>13</v>
       </c>
       <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="1:8" ht="50.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="50.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F19" s="11">
         <v>13</v>
       </c>
       <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" ht="54.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="54.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="25"/>
@@ -1985,19 +2025,19 @@
       <c r="G20" s="25"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E29" s="2"/>
     </row>
   </sheetData>

</xml_diff>